<commit_message>
Adding files and saving changes
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\Boot Camp  Data analytics program\Matplotlib-Homework-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65E8303-05E8-45A7-95F4-4FE64882B7DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879BCAF7-1BF3-4C4B-9A70-558A44F683A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF8E4552-2DDD-4BE8-8F3E-0C861481EDEE}"/>
   </bookViews>
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56A1A5A-667B-4E3A-9F67-2BEDCD03ED03}">
   <dimension ref="A2:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>